<commit_message>
Very Very small fix task 4
uncommented test for mapping
</commit_message>
<xml_diff>
--- a/data/reports/receipts_report.xlsx
+++ b/data/reports/receipts_report.xlsx
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>cb6ec5147cfa11ef83a11c9957818fb1</t>
+          <t>ca5977ea7cfc11efbcba1c9957818fb1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,7 +488,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cb6ec51d7cfa11ef896f1c9957818fb1</t>
+          <t>ca599f157cfc11ef90801c9957818fb1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>

<commit_message>
Revert "add task 7"
This reverts commit 46c584a9126e104c2bd125c4203cb31f40704b49.
</commit_message>
<xml_diff>
--- a/data/reports/receipts_report.xlsx
+++ b/data/reports/receipts_report.xlsx
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ef23f3c088ec11ef922d1c9957818fb1</t>
+          <t>f1e8112c844111ef87201c9957818fb1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,7 +488,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ef240dfb88ec11efa5c81c9957818fb1</t>
+          <t>f1e81155844111efa61b1c9957818fb1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>

<commit_message>
Reapply "add task 7"
This reverts commit 06e998f3ab5b0d28d75919db12c7a4e5ed9feab8.
</commit_message>
<xml_diff>
--- a/data/reports/receipts_report.xlsx
+++ b/data/reports/receipts_report.xlsx
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>f1e8112c844111ef87201c9957818fb1</t>
+          <t>ef23f3c088ec11ef922d1c9957818fb1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,7 +488,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>f1e81155844111efa61b1c9957818fb1</t>
+          <t>ef240dfb88ec11efa5c81c9957818fb1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>

<commit_message>
small fix main file
</commit_message>
<xml_diff>
--- a/data/reports/receipts_report.xlsx
+++ b/data/reports/receipts_report.xlsx
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ed0d6326896811efb02c1c9957818fb1</t>
+          <t>043701168a9011ef8b411c9957818fb1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,7 +488,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ed0d80a4896811efb4921c9957818fb1</t>
+          <t>0437013f8a9011ef8da11c9957818fb1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>

<commit_message>
add code from lesson
</commit_message>
<xml_diff>
--- a/data/reports/receipts_report.xlsx
+++ b/data/reports/receipts_report.xlsx
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>31bf3c339a4811efadd11c9957818fb1</t>
+          <t>9f6ff3449b1c11ef83fd1c9957818fb1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,7 +488,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>31bf3c5c9a4811ef9f861c9957818fb1</t>
+          <t>9f701a499b1c11ef94b41c9957818fb1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>

<commit_message>
small fix for auto tests
</commit_message>
<xml_diff>
--- a/data/reports/receipts_report.xlsx
+++ b/data/reports/receipts_report.xlsx
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>a147c7fc9f6c11efa2a61c9957818fb1</t>
+          <t>daf4b9f2a42311ef99831c9957818fb1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,7 +488,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>a147c8259f6c11ef844f1c9957818fb1</t>
+          <t>daf4ba1ba42311efa1751c9957818fb1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>

<commit_message>
fix naming file saved
</commit_message>
<xml_diff>
--- a/data/reports/receipts_report.xlsx
+++ b/data/reports/receipts_report.xlsx
@@ -456,7 +456,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>cfb41042a4f411ef85ed1c9957818fb1</t>
+          <t>a44bbea2a4f811efbd901c9957818fb1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,7 +488,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cfb4106ba4f411efa1ea1c9957818fb1</t>
+          <t>a44be5a4a4f811ef8c501c9957818fb1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>